<commit_message>
2020-01-16 diary of wenchia (#62)
</commit_message>
<xml_diff>
--- a/diaries/diary-wenchia_yang.xlsx
+++ b/diaries/diary-wenchia_yang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffbala/Desktop/Course/MSWE/2020 Winter/SWE 265P/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6627F438-2E6A-6E43-A859-114F2FB683D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F242D0-11E1-E143-9CF0-66FE255CEF83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-14160" windowWidth="38400" windowHeight="21600" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="-38400" yWindow="-13700" windowWidth="38400" windowHeight="21140" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>17:00 - 19:50</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
   <si>
     <t>1. Understood the course
@@ -88,6 +85,46 @@
   </si>
   <si>
     <t>I was shocked while building Jedit project because I haven't use ant to build my project before. After I bulit it, I got  tons of errors, and I have no idea where to begin fix them.</t>
+  </si>
+  <si>
+    <t>16:00 - 17:00</t>
+  </si>
+  <si>
+    <t>Me</t>
+  </si>
+  <si>
+    <t>Successfully build and run 3 open source projects</t>
+  </si>
+  <si>
+    <t>1. Successfully built and ran jedit
+2. Successfully built and ran google guava</t>
+  </si>
+  <si>
+    <t>1. Learned how to use ant build
+2. Learned how to use marven build
+3. Learned how to understand error message after built the project and tried to google it with more precise keywords</t>
+  </si>
+  <si>
+    <t>I tried multiple times to build jedit. Even though I think this project is a little bit outdated, I still enjoy the joy after successfully running it.</t>
+  </si>
+  <si>
+    <t>17:00 - 20:00</t>
+  </si>
+  <si>
+    <t>Solved bugs appeared in jpacman1 and jpacman2</t>
+  </si>
+  <si>
+    <t>1. Learned how to use different strategies to read code
+2. Tried to practice these strategies on the read-world projects
+3. Solved bugs before the professor showed the answer
+4. Learned industrial experience from googler(Ping Chen)</t>
+  </si>
+  <si>
+    <t>1. Understand different strategies to read code and practice them
+2. Industrial sharings from googler</t>
+  </si>
+  <si>
+    <t>The practice of solved buds is just like a competition. Though it might be a little bit stressed out, I still enjoy the moment that I found bugs.</t>
   </si>
 </sst>
 </file>
@@ -210,12 +247,23 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -226,7 +274,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -255,23 +303,29 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="9" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -594,7 +648,7 @@
   <dimension ref="A1:G122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -603,24 +657,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -689,25 +743,25 @@
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="10" t="s">
         <v>8</v>
       </c>
     </row>
@@ -719,38 +773,66 @@
         <v>14</v>
       </c>
       <c r="C10" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="E10" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="F10" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="G10" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="15" t="s">
+    </row>
+    <row r="11" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A11" s="12">
+        <v>43846</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8"/>
+      <c r="C11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+      <c r="A12" s="12">
+        <v>43846</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>

</xml_diff>

<commit_message>
0206 diary update wenchia (#275)
</commit_message>
<xml_diff>
--- a/diaries/diary-wenchia_yang.xlsx
+++ b/diaries/diary-wenchia_yang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffbala/Desktop/Course/MSWE/2020 Winter/SWE 265P/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0AD2656-BF14-0B4D-B2AC-9C72FE6BA886}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482CD74D-16CB-8F41-B51A-ABC3A3E0D684}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="-38400" yWindow="-13700" windowWidth="38400" windowHeight="21140" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="109">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -334,6 +334,54 @@
   </si>
   <si>
     <t>Feel Great!</t>
+  </si>
+  <si>
+    <t>20:00 - 21:00</t>
+  </si>
+  <si>
+    <t>To determine 2 features of homework 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discussed different features, we finally decided to use 'add new queries' and 'encryption' as our features.  </t>
+  </si>
+  <si>
+    <t>Learned how to use customers' or programmers' perspective to determine which features are needed to be updated.</t>
+  </si>
+  <si>
+    <t>Feel good!</t>
+  </si>
+  <si>
+    <t>To finish research of two features</t>
+  </si>
+  <si>
+    <t>Finished homework 2</t>
+  </si>
+  <si>
+    <t>1. Learned how to explain how to trace code to other group members.
+2. Learned how to understand and explain code to the team members.
+3. Learned how to write down my thought and understanding of the code.</t>
+  </si>
+  <si>
+    <t>Feel exhausted!</t>
+  </si>
+  <si>
+    <t>10:00 - 14:30</t>
+  </si>
+  <si>
+    <t>To read individual homework of week 4</t>
+  </si>
+  <si>
+    <t>1. Understood how UML diagram and Sequence Diagram work
+2. Tried examples in the Youtube videos</t>
+  </si>
+  <si>
+    <t>Learned how to use tools to draw UML and Sequence diagrams</t>
+  </si>
+  <si>
+    <t>Feel Proud!</t>
+  </si>
+  <si>
+    <t>13:00 - 14:30</t>
   </si>
 </sst>
 </file>
@@ -492,7 +540,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -556,6 +604,15 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -878,10 +935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
-  <dimension ref="A1:G123"/>
+  <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -890,24 +947,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -1366,32 +1423,74 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="21"/>
-    </row>
-    <row r="27" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="21"/>
-    </row>
-    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="21"/>
+    <row r="26" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A26" s="9">
+        <v>43865</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A27" s="22">
+        <v>43865</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="G27" s="21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A28" s="9">
+        <v>43867</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
@@ -2229,24 +2328,6 @@
       <c r="E121" s="20"/>
       <c r="F121" s="20"/>
       <c r="G121" s="21"/>
-    </row>
-    <row r="122" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A122" s="17"/>
-      <c r="B122" s="17"/>
-      <c r="C122" s="17"/>
-      <c r="D122" s="20"/>
-      <c r="E122" s="20"/>
-      <c r="F122" s="20"/>
-      <c r="G122" s="21"/>
-    </row>
-    <row r="123" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A123" s="17"/>
-      <c r="B123" s="17"/>
-      <c r="C123" s="17"/>
-      <c r="D123" s="20"/>
-      <c r="E123" s="20"/>
-      <c r="F123" s="20"/>
-      <c r="G123" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
0210 update diary, wen-chia (#300)
</commit_message>
<xml_diff>
--- a/diaries/diary-wenchia_yang.xlsx
+++ b/diaries/diary-wenchia_yang.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffbala/Desktop/Course/MSWE/2020 Winter/SWE 265P/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482CD74D-16CB-8F41-B51A-ABC3A3E0D684}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDD82C6-7635-9340-B102-895C13EA03AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-13700" windowWidth="38400" windowHeight="21140" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="113">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -382,6 +382,22 @@
   </si>
   <si>
     <t>13:00 - 14:30</t>
+  </si>
+  <si>
+    <t>1. Review homework 2 of group project
+2. Understand the concept of KEP and mental simulation.
+3. Midterm Review
+4. Industrial sharing</t>
+  </si>
+  <si>
+    <t>1. Understood KEP and metal simulation.
+2. Had a basic idea of the midterm</t>
+  </si>
+  <si>
+    <t>Learned how KEP concepts are important</t>
+  </si>
+  <si>
+    <t>Feel nervous because of the midterm! Feel not well-prepared for understanding every concept of previous lectures.</t>
   </si>
 </sst>
 </file>
@@ -937,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1492,14 +1508,28 @@
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="21"/>
+    <row r="29" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A29" s="9">
+        <v>43867</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="G29" s="18" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>

</xml_diff>

<commit_message>
update diary wenchia 0224
</commit_message>
<xml_diff>
--- a/diaries/diary-wenchia_yang.xlsx
+++ b/diaries/diary-wenchia_yang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffbala/Desktop/Course/MSWE/2020 Winter/SWE 265P/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDD82C6-7635-9340-B102-895C13EA03AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752BF801-AD53-2742-A401-8408C56FF109}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-13700" windowWidth="38400" windowHeight="21140" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="-38400" yWindow="-13700" windowWidth="38400" windowHeight="19760" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="167">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -398,6 +398,178 @@
   </si>
   <si>
     <t>Feel nervous because of the midterm! Feel not well-prepared for understanding every concept of previous lectures.</t>
+  </si>
+  <si>
+    <t>1. Understood who are stakeholders.
+2. Know the knowledge of seeing code with higher level.
+3. Realized the way to do when stucking.
+4. Leaned some examples to see the big picture.</t>
+  </si>
+  <si>
+    <t>1. Understand the concept of KEP(stakeholders, abstraction and do something when facing diffuculties).
+2. understood how to see the big picture of a project</t>
+  </si>
+  <si>
+    <t>1. Midterm
+2. More concepts of KEP.
+3. Concept of the big picture.</t>
+  </si>
+  <si>
+    <t>Feel so tired because of the midterm, and I think I lose some attention toward some lecture material.</t>
+  </si>
+  <si>
+    <t>15:00 - 15:20</t>
+  </si>
+  <si>
+    <t>Me, Junxian, Kaj</t>
+  </si>
+  <si>
+    <t>To get some feedback of assignment 2</t>
+  </si>
+  <si>
+    <t>We are struggling whether we should dive deep into another project.</t>
+  </si>
+  <si>
+    <t>Kaj told us to confirm whether our project is just a wapper or not. Learned some thought from Kaj because he told us that why a wrapper project owns over 10k lines of code. We then tried to dig deeper to the code to figure it out.</t>
+  </si>
+  <si>
+    <t>Feel bad because we didn't fully understand the entire project. And we need to find some proof to report Kaj whether our project is a wapper or not.</t>
+  </si>
+  <si>
+    <t>22:00 - 23:00</t>
+  </si>
+  <si>
+    <t>To find some essential parts in our project.</t>
+  </si>
+  <si>
+    <t>Find one potential candidate of essential feature but not sure if it is or not</t>
+  </si>
+  <si>
+    <t>I figured out that we had a wrong direction toward assignment 2, but still thought its somewhat hard to find 2 essential features in our projects.</t>
+  </si>
+  <si>
+    <t>Feel stressful!</t>
+  </si>
+  <si>
+    <t>10:00 - 11:00</t>
+  </si>
+  <si>
+    <t>To report our discussion and get feedback from Kaj</t>
+  </si>
+  <si>
+    <t>We still cannot garauntee that our project is just a wrapper, but Kaj told us we should prepare more for dive deeper into the core c++ project.</t>
+  </si>
+  <si>
+    <t>I had some picture of how we should address assignment 2 and had more understood toward our project.</t>
+  </si>
+  <si>
+    <t>Me, Junxian, Zihua, Craig</t>
+  </si>
+  <si>
+    <t>To understand the detail mechanism behind a database.</t>
+  </si>
+  <si>
+    <t>Have more understand toward our realm-core project structure and understand the basic mechanism of database.</t>
+  </si>
+  <si>
+    <t>Though my friend's sharing, I learned the process of building a database step by step. Even though realm might use some different mechanism, it still helpful to understand the standard steps.</t>
+  </si>
+  <si>
+    <t>21:00 - 23:00</t>
+  </si>
+  <si>
+    <t>To do some research of homework 3 and dispatch tasks to group members</t>
+  </si>
+  <si>
+    <t>Have a struture of doing the homework 3 and we try to finish each part.</t>
+  </si>
+  <si>
+    <t>I was in charge of finding key developers and fnd issues that we might be possibly solved it. Finding key developers is fun because I go through contributors LinkedIn file and figure out their roles.</t>
+  </si>
+  <si>
+    <t>To find out potential issues that we can solve</t>
+  </si>
+  <si>
+    <t>Successfully find 11 issues that we are interested or we might have a chance to solve.</t>
+  </si>
+  <si>
+    <t>Even though realm-java have issues less than 500, it still very hard for me to categorize them and figure out which one is suitable for us. Hence, I spent a lot of time tracking discussions in a lot issues and finally piked 11 results.</t>
+  </si>
+  <si>
+    <t>10:00 - 14:00</t>
+  </si>
+  <si>
+    <t>Successfully finished this section.</t>
+  </si>
+  <si>
+    <t>It's very hard for this part since I needed to read code, find potentially relating relationships, and try to give a solution.</t>
+  </si>
+  <si>
+    <t>14:00 - 17:00</t>
+  </si>
+  <si>
+    <t>To finish the entire homework 3</t>
+  </si>
+  <si>
+    <t>To finish the part in homework 3 of issue that we might be fixed</t>
+  </si>
+  <si>
+    <t>Successfully finished homework 3</t>
+  </si>
+  <si>
+    <t>Through this process, I understand more about our project than before. And for now, I have much more confidence to discuss our project with others.</t>
+  </si>
+  <si>
+    <t>1. Review homework 3 of group project
+2. Understand the concept of KEP, architecture and social context
+4. Industrial sharing</t>
+  </si>
+  <si>
+    <t>1. Understand the concept of KEP(know how things work, address knowledge deficincies and design elegant attractions).
+2. Understood the architecture of the project and had a real-time practice in class.
+3. Understood the concept of social context</t>
+  </si>
+  <si>
+    <t>I seldom to recovered architectre from other's project because my previous experience was that developers would at least havd some documentation or they would told you directly toward their code structure. In-class practice is really helpful, but I was wondering if this practice can also suitable for a big open-source project.</t>
+  </si>
+  <si>
+    <t>Feel not bad.</t>
+  </si>
+  <si>
+    <t>11:00 - 18:00</t>
+  </si>
+  <si>
+    <t>C++ is hard for me to read in the beginning, because I know nothing about it. After I figure out some keyword and relationship of files in c++, I had some progress of understanding project.</t>
+  </si>
+  <si>
+    <t>Have some basic understanding of this new project, and find 2 essential features.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To understand the entire codebase of realm-core and find 2 essential features in order to resubmit our assignment 2. </t>
+  </si>
+  <si>
+    <t>00:00 - 04:00</t>
+  </si>
+  <si>
+    <t>To do research toward 1 of the essential feature of assigment 2</t>
+  </si>
+  <si>
+    <t>Understand the higher level of the essential feature and try to make a report</t>
+  </si>
+  <si>
+    <t>I started to use pen and papper to draw UML diagram because the IDE cannot produce it for us in c++. After I go through the relationship in the feature, I had more confidence toward every relating classes. It also helped me understand the project more.</t>
+  </si>
+  <si>
+    <t>11:00 - 16:00</t>
+  </si>
+  <si>
+    <t>To finish the feature 1 in assignment 2</t>
+  </si>
+  <si>
+    <t>Finished most of it, and delegating other part to another group member (sequential diagram and its use case)</t>
+  </si>
+  <si>
+    <t>After explainning every detail toward relating classes in our essential feature 1, I feel more understanding toward how Real database work when creating table and using table.</t>
   </si>
 </sst>
 </file>
@@ -520,7 +692,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -548,6 +720,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -556,7 +737,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -629,6 +810,12 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -953,8 +1140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -963,24 +1150,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -1531,122 +1718,304 @@
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="21"/>
-    </row>
-    <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="21"/>
-    </row>
-    <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="17"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="21"/>
-    </row>
-    <row r="33" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="17"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="21"/>
-    </row>
-    <row r="34" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="17"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="21"/>
-    </row>
-    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="17"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="21"/>
-    </row>
-    <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="17"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="21"/>
-    </row>
-    <row r="37" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="17"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="21"/>
-    </row>
-    <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="17"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="21"/>
-    </row>
-    <row r="39" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="17"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="21"/>
-    </row>
-    <row r="40" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="17"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="21"/>
-    </row>
-    <row r="41" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="17"/>
-      <c r="B41" s="17"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="21"/>
-    </row>
-    <row r="42" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="17"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="21"/>
+    <row r="30" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="A30" s="9">
+        <v>43874</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="G30" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A31" s="9">
+        <v>43879</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="F31" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="G31" s="26" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A32" s="9">
+        <v>43879</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="G32" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A33" s="9">
+        <v>43880</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="G33" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A34" s="9">
+        <v>43880</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="G34" s="18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A35" s="9">
+        <v>43880</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="E35" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="F35" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="G35" s="18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A36" s="9">
+        <v>43881</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="F36" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G36" s="18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A37" s="9">
+        <v>43881</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="F37" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="G37" s="18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A38" s="9">
+        <v>43881</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="G38" s="18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="A39" s="9">
+        <v>43881</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="G39" s="18" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A40" s="9">
+        <v>43882</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="G40" s="18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="A41" s="9">
+        <v>43883</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="G41" s="18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A42" s="9">
+        <v>43883</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="E42" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="F42" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="G42" s="18" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>

</xml_diff>

<commit_message>
diary update wenchia 0227 (#416)
</commit_message>
<xml_diff>
--- a/diaries/diary-wenchia_yang.xlsx
+++ b/diaries/diary-wenchia_yang.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffbala/Desktop/Course/MSWE/2020 Winter/SWE 265P/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752BF801-AD53-2742-A401-8408C56FF109}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5BCD52-F255-E548-A157-DCB13AC16870}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-13700" windowWidth="38400" windowHeight="19760" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="188">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -570,6 +570,69 @@
   </si>
   <si>
     <t>After explainning every detail toward relating classes in our essential feature 1, I feel more understanding toward how Real database work when creating table and using table.</t>
+  </si>
+  <si>
+    <t>To think about about how to analyse architecture of the Realm</t>
+  </si>
+  <si>
+    <t>Find very few data about this</t>
+  </si>
+  <si>
+    <t>I used key word 'database architecture' for googling, but most results are related to 3-tier architecture. They are not what we want. Still workiing on it.</t>
+  </si>
+  <si>
+    <t>Feel unhappy!</t>
+  </si>
+  <si>
+    <t>To distribute the small tasks for every group members of assignment 4</t>
+  </si>
+  <si>
+    <t>Finish my part for finding 5 interesting issues.</t>
+  </si>
+  <si>
+    <t>I spent a lot of time tracing every discussions in one issue. Some are interesting because developers might propse nice solutions. Others are someone who don't understand deeply and just wanna answers. They might not be a real issue.</t>
+  </si>
+  <si>
+    <t>Feel intersting!</t>
+  </si>
+  <si>
+    <t>To understand the structure of a database</t>
+  </si>
+  <si>
+    <t>Have a basic understanding of how components work in a database</t>
+  </si>
+  <si>
+    <t>21:00 - 24:00</t>
+  </si>
+  <si>
+    <t>To understand the architecture of realm-core project</t>
+  </si>
+  <si>
+    <t>Have sucessfully understand the fundemental architecture of realm-core</t>
+  </si>
+  <si>
+    <t>I asked my roomate who took a database course last quarter to get a basic understand of components in a database. He gave me some keyword and references to study. It's really helpful, and I finally can understand the code structure in the realm-cre project.</t>
+  </si>
+  <si>
+    <t>We had some debates for some components in our project, but we finally had a conclusion toward the project. Interestingly, when we know nothing about the architecture, we thought a database is too hard for us. After we had a blueprint for understanding the project stucture, it became clearer to us.</t>
+  </si>
+  <si>
+    <t>Feel proud!</t>
+  </si>
+  <si>
+    <t>Feel relief!</t>
+  </si>
+  <si>
+    <t>13:00 - 15:00</t>
+  </si>
+  <si>
+    <t>To integrate every part into final assignment 4</t>
+  </si>
+  <si>
+    <t>Have successfully finished the assignment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We found how to cowork together everytime we finished the assignment. Even though we think every assignment is still not that easy, we still have ourr way to finish it. </t>
   </si>
 </sst>
 </file>
@@ -737,7 +800,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -818,6 +881,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1140,8 +1209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2017,50 +2086,120 @@
         <v>102</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="17"/>
-      <c r="B43" s="17"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="21"/>
-    </row>
-    <row r="44" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="17"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="21"/>
-    </row>
-    <row r="45" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="17"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="21"/>
-    </row>
-    <row r="46" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="17"/>
-      <c r="B46" s="17"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="21"/>
-    </row>
-    <row r="47" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="17"/>
-      <c r="B47" s="17"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="21"/>
+    <row r="43" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A43" s="9">
+        <v>43886</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="E43" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="F43" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="G43" s="18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="A44" s="9">
+        <v>43886</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="E44" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="F44" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="G44" s="18" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="A45" s="9">
+        <v>43887</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="G45" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="A46" s="28">
+        <v>43887</v>
+      </c>
+      <c r="B46" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="C46" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D46" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="E46" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="F46" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G46" s="26" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A47" s="9">
+        <v>43888</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="E47" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="F47" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="G47" s="18" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="17"/>

</xml_diff>

<commit_message>
wenchia diary update 0228
</commit_message>
<xml_diff>
--- a/diaries/diary-wenchia_yang.xlsx
+++ b/diaries/diary-wenchia_yang.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffbala/Desktop/Course/MSWE/2020 Winter/SWE 265P/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5BCD52-F255-E548-A157-DCB13AC16870}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D149DE22-8425-B54B-9582-8B25E780DC18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-13700" windowWidth="38400" windowHeight="19760" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="196">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -633,6 +633,34 @@
   </si>
   <si>
     <t xml:space="preserve">We found how to cowork together everytime we finished the assignment. Even though we think every assignment is still not that easy, we still have ourr way to finish it. </t>
+  </si>
+  <si>
+    <t>1. Review homework 4 of group project
+2. Understand the concept of KEP and design pattern
+3. Industrial sharing</t>
+  </si>
+  <si>
+    <t>1. Able to understand our project more
+2. Understand the concept of KEP(invest now to save effort later, socially embed and reinforce and use analogy)
+3. Have genenal concept of design pattern and in-class practice with strategy pattern</t>
+  </si>
+  <si>
+    <t>Undestood the benefits of design pattern even though it seems to be a little bit complex for a small project. However, for our project, I see the benefits of using design patterns. It's easier to understand the code because developers are following he nameing convention.</t>
+  </si>
+  <si>
+    <t>17:00 - 18:00</t>
+  </si>
+  <si>
+    <t>To learn strategy pattern and pracrice it with an actul code</t>
+  </si>
+  <si>
+    <t>Sucessfully made a small example and implented with strategy pattern</t>
+  </si>
+  <si>
+    <t>It's not that hard if you understand the definition, relationship and implementation of the design pattern. I tried to use different example other than the Duck example. It's really helpful.</t>
+  </si>
+  <si>
+    <t>Feel proud.</t>
   </si>
 </sst>
 </file>
@@ -880,13 +908,13 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="9" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1209,8 +1237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1219,24 +1247,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -2156,13 +2184,13 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="153" x14ac:dyDescent="0.2">
-      <c r="A46" s="28">
+      <c r="A46" s="27">
         <v>43887</v>
       </c>
-      <c r="B46" s="29" t="s">
+      <c r="B46" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="C46" s="29" t="s">
+      <c r="C46" s="28" t="s">
         <v>31</v>
       </c>
       <c r="D46" s="25" t="s">
@@ -2201,23 +2229,51 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="17"/>
-      <c r="B48" s="17"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="20"/>
-      <c r="G48" s="21"/>
-    </row>
-    <row r="49" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="17"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
-      <c r="G49" s="21"/>
+    <row r="48" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+      <c r="A48" s="9">
+        <v>43888</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="F48" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="G48" s="18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A49" s="9">
+        <v>43889</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D49" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="E49" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="F49" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="G49" s="18" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="50" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="17"/>

</xml_diff>

<commit_message>
diary update wenchia 0303
</commit_message>
<xml_diff>
--- a/diaries/diary-wenchia_yang.xlsx
+++ b/diaries/diary-wenchia_yang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffbala/Desktop/Course/MSWE/2020 Winter/SWE 265P/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D149DE22-8425-B54B-9582-8B25E780DC18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35AC44C0-A871-CB4D-97C7-2A3B53E9DF92}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-13700" windowWidth="38400" windowHeight="19760" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="208">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -661,6 +661,42 @@
   </si>
   <si>
     <t>Feel proud.</t>
+  </si>
+  <si>
+    <t>11:00 - 12:00</t>
+  </si>
+  <si>
+    <t>To learn observer pattern and pracrice it with an actul code</t>
+  </si>
+  <si>
+    <t>Sucessfully made two small examples and implented with observer pattern</t>
+  </si>
+  <si>
+    <t>The example code from the youtube website is not that practical, so I implemented with another example by using event listener. This is more like we will code in the real world situatin.</t>
+  </si>
+  <si>
+    <t>To learn decorator pattern and pracrice it with an actul code</t>
+  </si>
+  <si>
+    <t>Sucessfully made two small examples and implented with decorator pattern</t>
+  </si>
+  <si>
+    <t>Again, the example code from te Youtube isn't good as other resource from other website. Thus, I implemented two examples. The other one is clearer than the previous example.</t>
+  </si>
+  <si>
+    <t>17:00 - 18:30</t>
+  </si>
+  <si>
+    <t>To learn factory and abstract facory pattern and pracrice them with an actul code</t>
+  </si>
+  <si>
+    <t>Sucessfully made two small examples and implented with factory and abstract factory patterns</t>
+  </si>
+  <si>
+    <t>Feel useful!</t>
+  </si>
+  <si>
+    <t>This time, I implemented with the pattern by myself and made up some real world situations. Factory patterns are useful and thet often implemented by many application. I'm not unfamiliar with them.</t>
   </si>
 </sst>
 </file>
@@ -1237,8 +1273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2275,32 +2311,74 @@
         <v>195</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="17"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="21"/>
-    </row>
-    <row r="51" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" s="17"/>
-      <c r="B51" s="17"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="21"/>
-    </row>
-    <row r="52" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" s="17"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="17"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
-      <c r="G52" s="21"/>
+    <row r="50" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A50" s="9">
+        <v>43890</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D50" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="E50" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="F50" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="G50" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A51" s="9">
+        <v>43891</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D51" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="E51" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="F51" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="G51" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A52" s="9">
+        <v>43892</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D52" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="E52" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="F52" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="G52" s="18" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="53" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="17"/>

</xml_diff>